<commit_message>
Uploading two new scripts for pipeline and have updated genetic information spreadsheet to correct an incorrect genera name.
One script removes trailing spaces from multiple sequence alignment files to allow visualisation and manual editing of alignments in Geneious. The second script uses iqtree to make gene trees from multiple sequence alignments using iqtree.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/20240708_Orthofinder Results/Results_Jul07/Orthogroups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/2024_Orthofinder Results/Results_Jul07/Orthogroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53BE59D1-ADB2-4483-961B-4315C26E6FF8}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7944BF1C-D7E3-4A84-B541-BDC533CAEA97}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2184" yWindow="2316" windowWidth="17280" windowHeight="10104" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
+    <workbookView minimized="1" xWindow="5784" yWindow="708" windowWidth="17292" windowHeight="11856" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Orthogroups" sheetId="2" r:id="rId1"/>
@@ -17523,12 +17523,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -17543,8 +17549,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18147,9 +18154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F490DB99-BC92-4467-91FC-387E3D8437EE}">
   <dimension ref="A1:AT472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO195" sqref="AO195"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27889,143 +27896,143 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>2678</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>2679</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>2680</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="1" t="s">
         <v>2682</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="1" t="s">
         <v>2681</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="1" t="s">
         <v>2683</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" s="1" t="s">
         <v>2684</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="1" t="s">
         <v>2685</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70" s="1" t="s">
         <v>2686</v>
       </c>
-      <c r="J70" t="s">
+      <c r="J70" s="1" t="s">
         <v>2690</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K70" s="1" t="s">
         <v>2691</v>
       </c>
-      <c r="L70" t="s">
+      <c r="L70" s="1" t="s">
         <v>2692</v>
       </c>
-      <c r="M70" t="s">
+      <c r="M70" s="1" t="s">
         <v>2693</v>
       </c>
-      <c r="N70" t="s">
+      <c r="N70" s="1" t="s">
         <v>2694</v>
       </c>
-      <c r="O70" t="s">
+      <c r="O70" s="1" t="s">
         <v>2695</v>
       </c>
-      <c r="P70" t="s">
+      <c r="P70" s="1" t="s">
         <v>2697</v>
       </c>
-      <c r="Q70" t="s">
+      <c r="Q70" s="1" t="s">
         <v>2698</v>
       </c>
-      <c r="R70" t="s">
+      <c r="R70" s="1" t="s">
         <v>2699</v>
       </c>
-      <c r="S70" t="s">
+      <c r="S70" s="1" t="s">
         <v>2700</v>
       </c>
-      <c r="T70" t="s">
+      <c r="T70" s="1" t="s">
         <v>2701</v>
       </c>
-      <c r="U70" t="s">
+      <c r="U70" s="1" t="s">
         <v>2706</v>
       </c>
-      <c r="V70" t="s">
+      <c r="V70" s="1" t="s">
         <v>2707</v>
       </c>
-      <c r="W70" t="s">
+      <c r="W70" s="1" t="s">
         <v>2708</v>
       </c>
-      <c r="X70" t="s">
+      <c r="X70" s="1" t="s">
         <v>2709</v>
       </c>
-      <c r="Y70" t="s">
+      <c r="Y70" s="1" t="s">
         <v>2703</v>
       </c>
-      <c r="Z70" t="s">
+      <c r="Z70" s="1" t="s">
         <v>2704</v>
       </c>
-      <c r="AA70" t="s">
+      <c r="AA70" s="1" t="s">
         <v>2705</v>
       </c>
-      <c r="AB70" t="s">
+      <c r="AB70" s="1" t="s">
         <v>2696</v>
       </c>
-      <c r="AC70" t="s">
+      <c r="AC70" s="1" t="s">
         <v>2688</v>
       </c>
-      <c r="AD70" t="s">
+      <c r="AD70" s="1" t="s">
         <v>2702</v>
       </c>
-      <c r="AE70" t="s">
+      <c r="AE70" s="1" t="s">
         <v>2710</v>
       </c>
-      <c r="AF70" t="s">
+      <c r="AF70" s="1" t="s">
         <v>2689</v>
       </c>
-      <c r="AG70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AH70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AI70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AJ70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AK70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AL70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AM70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AN70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AO70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AP70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AQ70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR70" t="s">
-        <v>200</v>
-      </c>
-      <c r="AS70" t="s">
+      <c r="AG70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AH70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AK70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AN70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AP70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR70" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS70" s="1" t="s">
         <v>2687</v>
       </c>
-      <c r="AT70" t="s">
+      <c r="AT70" s="1" t="s">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating as I have progressed work on another genome (checking annotations)
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="203" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7944BF1C-D7E3-4A84-B541-BDC533CAEA97}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5784" yWindow="708" windowWidth="17292" windowHeight="11856" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
+    <workbookView minimized="1" xWindow="8208" yWindow="144" windowWidth="14832" windowHeight="13632" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Orthogroups" sheetId="2" r:id="rId1"/>
@@ -18154,9 +18154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F490DB99-BC92-4467-91FC-387E3D8437EE}">
   <dimension ref="A1:AT472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P63" sqref="P63"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated 'Manual Check' Spreadsheet having started manual check for TRBIV genome.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="203" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7944BF1C-D7E3-4A84-B541-BDC533CAEA97}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8208" yWindow="144" windowWidth="14832" windowHeight="13632" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Orthogroups" sheetId="2" r:id="rId1"/>
@@ -18154,9 +18154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F490DB99-BC92-4467-91FC-387E3D8437EE}">
   <dimension ref="A1:AT472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO4" sqref="AO4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Have competed annotation checks for MN803438, LS484712 and MF599468.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="203" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7944BF1C-D7E3-4A84-B541-BDC533CAEA97}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Orthogroups" sheetId="2" r:id="rId1"/>
@@ -18154,9 +18154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F490DB99-BC92-4467-91FC-387E3D8437EE}">
   <dimension ref="A1:AT472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR2" sqref="AR2:AR26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Annotation check (manual) now completed for 3 additional genomes.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/2024_Orthofinder Results/Results_Jul07/Orthogroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7944BF1C-D7E3-4A84-B541-BDC533CAEA97}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE2F659F-1DFB-48C1-A956-17073D064777}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Orthogroups" sheetId="2" r:id="rId1"/>
@@ -18155,8 +18155,8 @@
   <dimension ref="A1:AT472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR2" sqref="AR2:AR26"/>
+      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AT2" sqref="AT2:AT25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18197,7 +18197,7 @@
     <col min="35" max="35" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="73.44140625" customWidth="1"/>
     <col min="37" max="37" width="45.5546875" customWidth="1"/>
-    <col min="38" max="38" width="28.88671875" customWidth="1"/>
+    <col min="38" max="38" width="44" customWidth="1"/>
     <col min="39" max="39" width="38.33203125" customWidth="1"/>
     <col min="40" max="40" width="61.5546875" customWidth="1"/>
     <col min="41" max="41" width="50" customWidth="1"/>

</xml_diff>

<commit_message>
Have finished annotating FV3 genome.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -18155,8 +18155,8 @@
   <dimension ref="A1:AT472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AT2" sqref="AT2:AT25"/>
+      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Finished annotation check (manual) for second iridovirus genome.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="205" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE2F659F-1DFB-48C1-A956-17073D064777}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Orthogroups" sheetId="2" r:id="rId1"/>
@@ -18155,8 +18155,8 @@
   <dimension ref="A1:AT472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR7" sqref="AR7"/>
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AM18" sqref="AM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated date on manual annotation check document.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="205" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE2F659F-1DFB-48C1-A956-17073D064777}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Orthogroups" sheetId="2" r:id="rId1"/>
@@ -18155,8 +18155,8 @@
   <dimension ref="A1:AT472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM18" sqref="AM18"/>
+      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR22" sqref="AR22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Begun manual re-annotation of MG570131
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/2024_Orthofinder Results/Results_Jul07/Orthogroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE2F659F-1DFB-48C1-A956-17073D064777}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E73BA17-3A15-431D-9180-645F97EA104B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
@@ -18155,8 +18155,8 @@
   <dimension ref="A1:AT472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP2" sqref="AP2:AP27"/>
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18190,7 +18190,7 @@
     <col min="28" max="28" width="67.5546875" customWidth="1"/>
     <col min="29" max="29" width="66.88671875" customWidth="1"/>
     <col min="30" max="30" width="60.109375" customWidth="1"/>
-    <col min="31" max="31" width="45" customWidth="1"/>
+    <col min="31" max="31" width="52.33203125" customWidth="1"/>
     <col min="32" max="32" width="51.6640625" customWidth="1"/>
     <col min="33" max="33" width="35.21875" customWidth="1"/>
     <col min="34" max="34" width="38.77734375" customWidth="1"/>

</xml_diff>

<commit_message>
I went back and resolved some issues I had highlighted earlier in the manual checking process.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/2024_Orthofinder Results/Results_Jul07/Orthogroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E73BA17-3A15-431D-9180-645F97EA104B}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="8_{2B205E00-3B37-4A84-A0E4-0BFE2F278F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38EED349-D17E-4378-A655-CF55BEBCDB0C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A74813FE-C142-431E-93FA-E3E9EB22F48C}"/>
   </bookViews>
@@ -18154,9 +18154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F490DB99-BC92-4467-91FC-387E3D8437EE}">
   <dimension ref="A1:AT472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF10" sqref="AF10"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ34" sqref="AJ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Started manual annotations for OQ475017.
</commit_message>
<xml_diff>
--- a/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
+++ b/2024_Orthofinder Results/Results_Jul07/Orthogroups/Orthogroups_adapted for analysis and columns rearranged_20240807.xlsx
@@ -18154,9 +18154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F490DB99-BC92-4467-91FC-387E3D8437EE}">
   <dimension ref="A1:AT472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ34" sqref="AJ34"/>
+    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>